<commit_message>
Develop: reset playerModel structure and calculate the total number of each attribute
</commit_message>
<xml_diff>
--- a/src/uploads/2023-08-14.xlsx
+++ b/src/uploads/2023-08-14.xlsx
@@ -1138,8 +1138,8 @@
   <sheetPr/>
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1285,13 +1285,13 @@
         <v>23</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -1306,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
@@ -1315,16 +1315,16 @@
         <v>0</v>
       </c>
       <c r="L3" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M3" s="1">
         <v>0</v>
       </c>
       <c r="N3" s="1">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="O3" s="1">
-        <v>6.2</v>
+        <v>0</v>
       </c>
       <c r="P3" s="1">
         <v>0</v>
@@ -1339,10 +1339,10 @@
         <v>0</v>
       </c>
       <c r="T3" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="U3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3" s="1">
         <v>0</v>
@@ -1353,13 +1353,13 @@
         <v>24</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -1374,7 +1374,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
@@ -1383,16 +1383,16 @@
         <v>0</v>
       </c>
       <c r="L4" s="1">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M4" s="1">
         <v>0</v>
       </c>
       <c r="N4" s="1">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>6.2</v>
       </c>
       <c r="P4" s="1">
         <v>0</v>
@@ -1407,10 +1407,10 @@
         <v>0</v>
       </c>
       <c r="T4" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4" s="1">
         <v>0</v>

</xml_diff>